<commit_message>
Move compiler.py to assemble/ .
</commit_message>
<xml_diff>
--- a/doc/控制器.xlsx
+++ b/doc/控制器.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="寄存器定义" sheetId="2" r:id="rId1"/>
@@ -624,6 +624,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -651,10 +655,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1111,11 +1111,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1123,7 +1123,7 @@
     <col min="4" max="4" width="10.1640625" style="16" customWidth="1"/>
     <col min="5" max="8" width="8.83203125" style="16"/>
     <col min="9" max="9" width="15.1640625" style="16" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="16"/>
+    <col min="10" max="10" width="11.5" style="16" customWidth="1"/>
     <col min="11" max="11" width="21.1640625" style="16" customWidth="1"/>
     <col min="12" max="12" width="16" style="16" customWidth="1"/>
     <col min="13" max="13" width="13.4140625" style="16" customWidth="1"/>
@@ -1132,35 +1132,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
     </row>
     <row r="3" spans="1:16" ht="28">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="17" t="s">
         <v>12</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="35" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1">
@@ -1247,7 +1247,7 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="34"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -1292,7 +1292,7 @@
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="34"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -1337,7 +1337,7 @@
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="34"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -1382,7 +1382,7 @@
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="34"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="3">
         <v>23</v>
       </c>
@@ -1427,7 +1427,7 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="34"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="5">
         <v>29</v>
       </c>
@@ -1472,7 +1472,7 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="35" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="3">
@@ -1519,7 +1519,7 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="34"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="5">
         <v>20</v>
       </c>
@@ -1564,7 +1564,7 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="35" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="3">
@@ -1611,7 +1611,7 @@
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="34"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="3">
         <v>22</v>
       </c>
@@ -1656,7 +1656,7 @@
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="34"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="5">
         <v>30</v>
       </c>
@@ -1701,7 +1701,7 @@
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="35" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="3">
@@ -1748,7 +1748,7 @@
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="34"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="3">
         <v>7</v>
       </c>
@@ -1793,7 +1793,7 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="34"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="3">
         <v>8</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="34"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="3">
         <v>9</v>
       </c>
@@ -1883,7 +1883,7 @@
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="34"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="3">
         <v>11</v>
       </c>
@@ -1928,7 +1928,7 @@
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="34"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="3">
         <v>26</v>
       </c>
@@ -1973,7 +1973,7 @@
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="34"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="5">
         <v>27</v>
       </c>
@@ -2018,7 +2018,7 @@
       </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="3">
@@ -2065,7 +2065,7 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="34"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="5">
         <v>28</v>
       </c>
@@ -2110,7 +2110,7 @@
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="3">
@@ -2157,7 +2157,7 @@
       </c>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="34"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="3">
         <v>16</v>
       </c>
@@ -2202,7 +2202,7 @@
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="34"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="3">
         <v>17</v>
       </c>
@@ -2247,7 +2247,7 @@
       </c>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="34"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="5">
         <v>18</v>
       </c>
@@ -2292,7 +2292,7 @@
       </c>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="35" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="3">
@@ -2339,7 +2339,7 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="34"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="3">
         <v>13</v>
       </c>
@@ -2384,7 +2384,7 @@
       </c>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="34"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="3">
         <v>14</v>
       </c>
@@ -2429,7 +2429,7 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="34"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="3">
         <v>24</v>
       </c>
@@ -2474,7 +2474,7 @@
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="34"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="3">
         <v>31</v>
       </c>
@@ -2519,7 +2519,7 @@
       </c>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="34"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="5">
         <v>25</v>
       </c>
@@ -2634,9 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C045E36-7B6A-4984-B732-FE0758B948D8}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
@@ -2652,10 +2650,10 @@
       <c r="B1" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="38">
-        <v>0</v>
-      </c>
-      <c r="D1" s="40" t="s">
+      <c r="C1" s="40">
+        <v>0</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>89</v>
       </c>
       <c r="E1" s="20"/>
@@ -2675,8 +2673,8 @@
       <c r="B2" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
@@ -2688,13 +2686,13 @@
       <c r="M2" s="20"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="33" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="22">
         <v>0</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="34">
         <v>2</v>
       </c>
       <c r="D3" s="10">

</xml_diff>

<commit_message>
Add ALU and Mux6, 控制器的excel加入了ALUOp
</commit_message>
<xml_diff>
--- a/doc/控制器.xlsx
+++ b/doc/控制器.xlsx
@@ -1,34 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangwx/Programs/ComputerOrganization/SAOestCPU/doc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8220" windowWidth="25600" windowHeight="7780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="寄存器定义" sheetId="2" r:id="rId1"/>
     <sheet name="Controller" sheetId="1" r:id="rId2"/>
     <sheet name="BranchController" sheetId="3" r:id="rId3"/>
     <sheet name="ALUOp" sheetId="4" r:id="rId4"/>
+    <sheet name="ALUFlag" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="105">
   <si>
     <t>寄存器</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -339,17 +345,38 @@
   <si>
     <t>PCOffset</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALUFlag</t>
+  </si>
+  <si>
+    <t>Flag Symbol</t>
+  </si>
+  <si>
+    <t>Z (Zero Flag)</t>
+  </si>
+  <si>
+    <t>C (Carry Flag)</t>
+  </si>
+  <si>
+    <t>S (Sign Flag)</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>O (Overflow Flag)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -368,7 +395,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -400,6 +427,13 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -544,7 +578,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -628,6 +662,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -657,8 +697,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 6" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -693,7 +733,7 @@
         <xdr:cNvPr id="3" name="直接连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FCE7D1A-8146-4B2C-8BF5-1F1E1E5E6C9F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FCE7D1A-8146-4B2C-8BF5-1F1E1E5E6C9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -743,7 +783,7 @@
         <xdr:cNvPr id="5" name="直接连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2262EF2A-6BE7-4BAE-B7BB-F24298545F56}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2262EF2A-6BE7-4BAE-B7BB-F24298545F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1040,20 +1080,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.4140625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
@@ -1069,7 +1109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -1077,7 +1117,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -1085,7 +1125,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -1093,7 +1133,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -1108,17 +1148,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="10.1640625" style="16" customWidth="1"/>
     <col min="5" max="8" width="8.83203125" style="16"/>
@@ -1126,41 +1166,41 @@
     <col min="10" max="10" width="11.5" style="16" customWidth="1"/>
     <col min="11" max="11" width="21.1640625" style="16" customWidth="1"/>
     <col min="12" max="12" width="16" style="16" customWidth="1"/>
-    <col min="13" max="13" width="13.4140625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="16" customWidth="1"/>
     <col min="14" max="14" width="13.83203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="12.4140625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-    </row>
-    <row r="3" spans="1:16" ht="28">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+    </row>
+    <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.2">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="17" t="s">
         <v>12</v>
       </c>
@@ -1199,8 +1239,8 @@
       </c>
       <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1">
@@ -1246,8 +1286,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="36"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="38"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -1291,8 +1331,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="36"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="38"/>
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -1336,8 +1376,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="36"/>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="38"/>
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -1381,8 +1421,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="36"/>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="38"/>
       <c r="B8" s="3">
         <v>23</v>
       </c>
@@ -1426,8 +1466,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="36"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="38"/>
       <c r="B9" s="5">
         <v>29</v>
       </c>
@@ -1471,8 +1511,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="35" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="3">
@@ -1518,8 +1558,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="36"/>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="38"/>
       <c r="B11" s="5">
         <v>20</v>
       </c>
@@ -1563,8 +1603,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="35" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="3">
@@ -1610,8 +1650,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="36"/>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="38"/>
       <c r="B13" s="3">
         <v>22</v>
       </c>
@@ -1655,8 +1695,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="36"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="38"/>
       <c r="B14" s="5">
         <v>30</v>
       </c>
@@ -1700,8 +1740,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="35" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="37" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="3">
@@ -1747,8 +1787,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="36"/>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="38"/>
       <c r="B16" s="3">
         <v>7</v>
       </c>
@@ -1792,8 +1832,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="36"/>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="38"/>
       <c r="B17" s="3">
         <v>8</v>
       </c>
@@ -1837,8 +1877,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="36"/>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="38"/>
       <c r="B18" s="3">
         <v>9</v>
       </c>
@@ -1882,8 +1922,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="36"/>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="38"/>
       <c r="B19" s="3">
         <v>11</v>
       </c>
@@ -1927,8 +1967,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="36"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="38"/>
       <c r="B20" s="3">
         <v>26</v>
       </c>
@@ -1972,8 +2012,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="36"/>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="38"/>
       <c r="B21" s="5">
         <v>27</v>
       </c>
@@ -2017,8 +2057,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="35" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="37" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="3">
@@ -2064,8 +2104,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="36"/>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="38"/>
       <c r="B23" s="5">
         <v>28</v>
       </c>
@@ -2109,8 +2149,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="35" t="s">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="3">
@@ -2156,8 +2196,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="36"/>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="38"/>
       <c r="B25" s="3">
         <v>16</v>
       </c>
@@ -2201,8 +2241,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="36"/>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="38"/>
       <c r="B26" s="3">
         <v>17</v>
       </c>
@@ -2246,8 +2286,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="36"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="38"/>
       <c r="B27" s="5">
         <v>18</v>
       </c>
@@ -2291,8 +2331,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="35" t="s">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="37" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="3">
@@ -2338,8 +2378,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="36"/>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="38"/>
       <c r="B29" s="3">
         <v>13</v>
       </c>
@@ -2383,8 +2423,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
-      <c r="A30" s="36"/>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="38"/>
       <c r="B30" s="3">
         <v>14</v>
       </c>
@@ -2428,8 +2468,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="36"/>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="38"/>
       <c r="B31" s="3">
         <v>24</v>
       </c>
@@ -2473,8 +2513,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="36"/>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="38"/>
       <c r="B32" s="3">
         <v>31</v>
       </c>
@@ -2518,8 +2558,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="36"/>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="38"/>
       <c r="B33" s="5">
         <v>25</v>
       </c>
@@ -2563,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
         <v>78</v>
       </c>
@@ -2631,29 +2671,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C045E36-7B6A-4984-B732-FE0758B948D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.4140625" customWidth="1"/>
-    <col min="2" max="2" width="19.08203125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29" customHeight="1">
+    <row r="1" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="40">
-        <v>0</v>
-      </c>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="42">
+        <v>0</v>
+      </c>
+      <c r="D1" s="44" t="s">
         <v>89</v>
       </c>
       <c r="E1" s="20"/>
@@ -2666,15 +2706,15 @@
       <c r="L1" s="20"/>
       <c r="M1" s="20"/>
     </row>
-    <row r="2" spans="1:13" ht="39.5" customHeight="1">
+    <row r="2" spans="1:13" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
@@ -2685,7 +2725,7 @@
       <c r="L2" s="20"/>
       <c r="M2" s="20"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>51</v>
       </c>
@@ -2699,7 +2739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>52</v>
       </c>
@@ -2713,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>54</v>
       </c>
@@ -2727,7 +2767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>55</v>
       </c>
@@ -2741,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>57</v>
       </c>
@@ -2755,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>58</v>
       </c>
@@ -2769,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
         <v>60</v>
       </c>
@@ -2783,7 +2823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>94</v>
       </c>
@@ -2794,7 +2834,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="23">
         <v>1</v>
@@ -2803,7 +2843,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="24">
         <v>2</v>
@@ -2824,20 +2864,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9134E1-7BBF-4C70-B2CC-9F10822CA5EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.4140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>82</v>
       </c>
@@ -2845,7 +2885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -2853,7 +2893,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>27</v>
       </c>
@@ -2861,7 +2901,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>36</v>
       </c>
@@ -2869,7 +2909,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>40</v>
       </c>
@@ -2877,7 +2917,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>42</v>
       </c>
@@ -2885,7 +2925,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>45</v>
       </c>
@@ -2893,7 +2933,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>49</v>
       </c>
@@ -2901,7 +2941,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>47</v>
       </c>
@@ -2914,4 +2954,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="210" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement Controller and refine ALU.
</commit_message>
<xml_diff>
--- a/doc/控制器.xlsx
+++ b/doc/控制器.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangwx/Programs/ComputerOrganization/SAOestCPU/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yifan/Desktop/SAOestCPU/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-220" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="14400" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="寄存器定义" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="108">
   <si>
     <t>寄存器</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -366,6 +366,18 @@
   </si>
   <si>
     <t>O (Overflow Flag)</t>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0(1100)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZERO</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -376,7 +388,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -395,7 +407,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -432,7 +444,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -638,6 +650,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -653,6 +689,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -665,36 +704,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 6" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -730,7 +742,7 @@
         <xdr:cNvPr id="3" name="直接连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1FCE7D1A-8146-4B2C-8BF5-1F1E1E5E6C9F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FCE7D1A-8146-4B2C-8BF5-1F1E1E5E6C9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -780,7 +792,7 @@
         <xdr:cNvPr id="5" name="直接连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2262EF2A-6BE7-4BAE-B7BB-F24298545F56}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2262EF2A-6BE7-4BAE-B7BB-F24298545F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1078,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1131,11 +1143,19 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>1011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1100</v>
       </c>
     </row>
   </sheetData>
@@ -1148,11 +1168,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1172,36 +1192,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
     </row>
     <row r="3" spans="1:17" ht="28" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1220,10 +1240,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="36"/>
+      <c r="K3" s="40"/>
       <c r="L3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1242,13 +1262,13 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37">
-        <v>1</v>
-      </c>
-      <c r="C4" s="38" t="s">
+      <c r="B4" s="27">
+        <v>1</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -1270,7 +1290,7 @@
         <v>26</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>27</v>
@@ -1292,11 +1312,11 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="39">
+      <c r="A5" s="36"/>
+      <c r="B5" s="29">
         <v>2</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="30" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1340,11 +1360,11 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="39">
+      <c r="A6" s="36"/>
+      <c r="B6" s="29">
         <v>3</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="30" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1372,13 +1392,13 @@
         <v>27</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="O6" s="7">
         <v>3</v>
@@ -1388,11 +1408,11 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="39">
+      <c r="A7" s="36"/>
+      <c r="B7" s="29">
         <v>4</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="30" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1436,11 +1456,11 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="39">
+      <c r="A8" s="36"/>
+      <c r="B8" s="29">
         <v>23</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="30" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1484,11 +1504,11 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="41">
+      <c r="A9" s="36"/>
+      <c r="B9" s="31">
         <v>29</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="32" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -1515,8 +1535,8 @@
       <c r="K9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="7">
-        <v>0</v>
+      <c r="L9" s="7" t="s">
+        <v>106</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>30</v>
@@ -1532,13 +1552,13 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="29">
         <v>5</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="30" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -1582,11 +1602,11 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="41">
+      <c r="A11" s="36"/>
+      <c r="B11" s="31">
         <v>20</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="32" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -1630,13 +1650,13 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="29">
         <v>21</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="30" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -1680,11 +1700,11 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
-      <c r="B13" s="39">
+      <c r="A13" s="36"/>
+      <c r="B13" s="29">
         <v>22</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="30" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1728,11 +1748,11 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="41">
+      <c r="A14" s="36"/>
+      <c r="B14" s="31">
         <v>30</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="32" t="s">
         <v>48</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -1776,13 +1796,13 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="39">
+      <c r="B15" s="29">
         <v>6</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="30" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -1826,11 +1846,11 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="28"/>
-      <c r="B16" s="39">
+      <c r="A16" s="36"/>
+      <c r="B16" s="29">
         <v>7</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="30" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -1874,11 +1894,11 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
-      <c r="B17" s="39">
+      <c r="A17" s="36"/>
+      <c r="B17" s="29">
         <v>8</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="30" t="s">
         <v>54</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -1922,11 +1942,11 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
-      <c r="B18" s="39">
+      <c r="A18" s="36"/>
+      <c r="B18" s="29">
         <v>9</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="30" t="s">
         <v>55</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -1970,11 +1990,11 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="39">
+      <c r="A19" s="36"/>
+      <c r="B19" s="29">
         <v>11</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="30" t="s">
         <v>57</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -2018,11 +2038,11 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="39">
-        <v>26</v>
-      </c>
-      <c r="C20" s="40" t="s">
+      <c r="A20" s="36"/>
+      <c r="B20" s="29">
+        <v>26</v>
+      </c>
+      <c r="C20" s="30" t="s">
         <v>58</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -2066,11 +2086,11 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="28"/>
-      <c r="B21" s="41">
+      <c r="A21" s="36"/>
+      <c r="B21" s="31">
         <v>27</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="32" t="s">
         <v>60</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -2114,13 +2134,13 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="39">
+      <c r="B22" s="29">
         <v>10</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="30" t="s">
         <v>62</v>
       </c>
       <c r="D22" s="7">
@@ -2164,11 +2184,11 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="41">
+      <c r="A23" s="36"/>
+      <c r="B23" s="31">
         <v>28</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="32" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="7">
@@ -2212,13 +2232,13 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="39">
+      <c r="B24" s="29">
         <v>15</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="30" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -2262,11 +2282,11 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="28"/>
-      <c r="B25" s="39">
+      <c r="A25" s="36"/>
+      <c r="B25" s="29">
         <v>16</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="30" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -2310,11 +2330,11 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
-      <c r="B26" s="39">
+      <c r="A26" s="36"/>
+      <c r="B26" s="29">
         <v>17</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="30" t="s">
         <v>69</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -2358,11 +2378,11 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
-      <c r="B27" s="41">
+      <c r="A27" s="36"/>
+      <c r="B27" s="31">
         <v>18</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="32" t="s">
         <v>70</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -2406,13 +2426,13 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="39">
+      <c r="B28" s="29">
         <v>12</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="30" t="s">
         <v>72</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -2456,11 +2476,11 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
-      <c r="B29" s="39">
+      <c r="A29" s="36"/>
+      <c r="B29" s="29">
         <v>13</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="30" t="s">
         <v>73</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -2504,11 +2524,11 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
-      <c r="B30" s="39">
+      <c r="A30" s="36"/>
+      <c r="B30" s="29">
         <v>14</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="30" t="s">
         <v>74</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -2552,11 +2572,11 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
-      <c r="B31" s="39">
+      <c r="A31" s="36"/>
+      <c r="B31" s="29">
         <v>24</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D31" s="7" t="s">
@@ -2600,11 +2620,11 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
-      <c r="B32" s="39">
+      <c r="A32" s="36"/>
+      <c r="B32" s="29">
         <v>31</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="32" t="s">
         <v>76</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -2648,11 +2668,11 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="28"/>
-      <c r="B33" s="41">
+      <c r="A33" s="36"/>
+      <c r="B33" s="31">
         <v>25</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="32" t="s">
         <v>77</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -2699,10 +2719,10 @@
       <c r="A34" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="43">
+      <c r="B34" s="33">
         <v>19</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="34" t="s">
         <v>79</v>
       </c>
       <c r="D34" s="7" t="s">
@@ -2786,10 +2806,10 @@
       <c r="B1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="32">
-        <v>0</v>
-      </c>
-      <c r="D1" s="34" t="s">
+      <c r="C1" s="41">
+        <v>0</v>
+      </c>
+      <c r="D1" s="43" t="s">
         <v>89</v>
       </c>
       <c r="E1" s="9"/>
@@ -2809,8 +2829,8 @@
       <c r="B2" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="35"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -3107,6 +3127,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add ForwardUnit, adjust logic in RF, set a new RegDst '1111' standing for no RegDst in order to prevent conflict in ForwardUnit.
</commit_message>
<xml_diff>
--- a/doc/控制器.xlsx
+++ b/doc/控制器.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="14400" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="寄存器定义" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="109">
   <si>
     <t>寄存器</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -377,6 +377,10 @@
   </si>
   <si>
     <t>ZERO</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO USE(prevent from forward)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -742,7 +746,7 @@
         <xdr:cNvPr id="3" name="直接连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FCE7D1A-8146-4B2C-8BF5-1F1E1E5E6C9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1FCE7D1A-8146-4B2C-8BF5-1F1E1E5E6C9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -792,7 +796,7 @@
         <xdr:cNvPr id="5" name="直接连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2262EF2A-6BE7-4BAE-B7BB-F24298545F56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2262EF2A-6BE7-4BAE-B7BB-F24298545F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1090,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1151,11 +1155,19 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>1100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1111</v>
       </c>
     </row>
   </sheetData>
@@ -1169,10 +1181,10 @@
   <dimension ref="A2:Q34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix bugs in control signals.
</commit_message>
<xml_diff>
--- a/doc/控制器.xlsx
+++ b/doc/控制器.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="111">
   <si>
     <t>寄存器</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -364,10 +364,6 @@
   </si>
   <si>
     <t>0001</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>0(1100)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -461,12 +457,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -603,7 +605,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -660,36 +662,27 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -717,6 +710,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1165,7 +1177,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="4">
         <v>1100</v>
@@ -1173,7 +1185,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="6">
         <v>1111</v>
@@ -1190,10 +1202,10 @@
   <dimension ref="A2:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1213,36 +1225,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
     </row>
     <row r="3" spans="1:17" ht="28">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1261,10 +1273,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="40"/>
+      <c r="K3" s="37"/>
       <c r="L3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1283,13 +1295,13 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="27">
-        <v>1</v>
-      </c>
-      <c r="C4" s="28" t="s">
+      <c r="B4" s="26">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -1308,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>105</v>
@@ -1320,7 +1332,7 @@
         <v>28</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>28</v>
@@ -1333,11 +1345,11 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="36"/>
-      <c r="B5" s="29">
+      <c r="A5" s="33"/>
+      <c r="B5" s="28">
         <v>2</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1356,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>85</v>
@@ -1368,7 +1380,7 @@
         <v>28</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>30</v>
@@ -1381,11 +1393,11 @@
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="36"/>
-      <c r="B6" s="29">
+      <c r="A6" s="33"/>
+      <c r="B6" s="28">
         <v>3</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1404,7 +1416,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>85</v>
@@ -1416,7 +1428,7 @@
         <v>6</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>6</v>
@@ -1429,11 +1441,11 @@
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="36"/>
-      <c r="B7" s="29">
+      <c r="A7" s="33"/>
+      <c r="B7" s="28">
         <v>4</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1452,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>85</v>
@@ -1477,11 +1489,11 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="36"/>
-      <c r="B8" s="29">
+      <c r="A8" s="33"/>
+      <c r="B8" s="28">
         <v>23</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="29" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1500,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>86</v>
@@ -1525,11 +1537,11 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="36"/>
-      <c r="B9" s="31">
+      <c r="A9" s="33"/>
+      <c r="B9" s="30">
         <v>29</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="31" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -1548,7 +1560,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>86</v>
@@ -1573,13 +1585,13 @@
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="28">
         <v>5</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -1598,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>87</v>
@@ -1623,11 +1635,11 @@
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="36"/>
-      <c r="B11" s="31">
+      <c r="A11" s="33"/>
+      <c r="B11" s="30">
         <v>20</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="31" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -1646,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>88</v>
@@ -1671,13 +1683,13 @@
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="28">
         <v>21</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -1696,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>90</v>
@@ -1708,7 +1720,7 @@
         <v>30</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N12" s="7" t="s">
         <v>28</v>
@@ -1721,11 +1733,11 @@
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="36"/>
-      <c r="B13" s="29">
+      <c r="A13" s="33"/>
+      <c r="B13" s="28">
         <v>22</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="29" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1744,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>92</v>
@@ -1756,7 +1768,7 @@
         <v>30</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N13" s="7" t="s">
         <v>28</v>
@@ -1769,11 +1781,11 @@
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="36"/>
-      <c r="B14" s="31">
+      <c r="A14" s="33"/>
+      <c r="B14" s="30">
         <v>30</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -1792,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>91</v>
@@ -1804,7 +1816,7 @@
         <v>30</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N14" s="7" t="s">
         <v>28</v>
@@ -1817,13 +1829,13 @@
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="28">
         <v>6</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="29" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -1851,13 +1863,13 @@
         <v>26</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>26</v>
@@ -1867,11 +1879,11 @@
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="36"/>
-      <c r="B16" s="29">
+      <c r="A16" s="33"/>
+      <c r="B16" s="28">
         <v>7</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="29" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -1902,10 +1914,10 @@
         <v>53</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O16" s="7" t="s">
         <v>26</v>
@@ -1915,11 +1927,11 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="36"/>
-      <c r="B17" s="29">
+      <c r="A17" s="33"/>
+      <c r="B17" s="28">
         <v>8</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="29" t="s">
         <v>54</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -1950,10 +1962,10 @@
         <v>53</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O17" s="7" t="s">
         <v>26</v>
@@ -1963,11 +1975,11 @@
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="36"/>
-      <c r="B18" s="29">
+      <c r="A18" s="33"/>
+      <c r="B18" s="28">
         <v>9</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="29" t="s">
         <v>55</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -1998,10 +2010,10 @@
         <v>56</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O18" s="7" t="s">
         <v>26</v>
@@ -2011,11 +2023,11 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="36"/>
-      <c r="B19" s="29">
+      <c r="A19" s="33"/>
+      <c r="B19" s="28">
         <v>11</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="29" t="s">
         <v>57</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -2046,10 +2058,10 @@
         <v>53</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O19" s="7" t="s">
         <v>26</v>
@@ -2059,11 +2071,11 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="36"/>
-      <c r="B20" s="29">
-        <v>26</v>
-      </c>
-      <c r="C20" s="30" t="s">
+      <c r="A20" s="33"/>
+      <c r="B20" s="28">
+        <v>26</v>
+      </c>
+      <c r="C20" s="29" t="s">
         <v>58</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -2094,7 +2106,7 @@
         <v>53</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N20" s="7" t="s">
         <v>59</v>
@@ -2107,11 +2119,11 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="36"/>
-      <c r="B21" s="31">
+      <c r="A21" s="33"/>
+      <c r="B21" s="30">
         <v>27</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="31" t="s">
         <v>60</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -2142,10 +2154,10 @@
         <v>59</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O21" s="7" t="s">
         <v>26</v>
@@ -2155,13 +2167,13 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="28">
         <v>10</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="29" t="s">
         <v>62</v>
       </c>
       <c r="D22" s="7">
@@ -2180,7 +2192,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>86</v>
@@ -2198,18 +2210,18 @@
         <v>63</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="36"/>
-      <c r="B23" s="31">
+      <c r="A23" s="33"/>
+      <c r="B23" s="30">
         <v>28</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="31" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="7">
@@ -2228,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>86</v>
@@ -2246,20 +2258,20 @@
         <v>63</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="29">
+      <c r="B24" s="28">
         <v>15</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="29" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -2278,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J24" s="8" t="s">
         <v>84</v>
@@ -2290,7 +2302,7 @@
         <v>67</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N24" s="7" t="s">
         <v>28</v>
@@ -2303,11 +2315,11 @@
       </c>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="36"/>
-      <c r="B25" s="29">
+      <c r="A25" s="33"/>
+      <c r="B25" s="28">
         <v>16</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="29" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -2326,7 +2338,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>84</v>
@@ -2335,10 +2347,10 @@
         <v>26</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N25" s="7" t="s">
         <v>28</v>
@@ -2351,11 +2363,11 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="36"/>
-      <c r="B26" s="29">
+      <c r="A26" s="33"/>
+      <c r="B26" s="28">
         <v>17</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -2374,7 +2386,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>84</v>
@@ -2386,7 +2398,7 @@
         <v>28</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N26" s="7" t="s">
         <v>67</v>
@@ -2399,11 +2411,11 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="36"/>
-      <c r="B27" s="31">
+      <c r="A27" s="33"/>
+      <c r="B27" s="30">
         <v>18</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="31" t="s">
         <v>70</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -2422,7 +2434,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>84</v>
@@ -2434,7 +2446,7 @@
         <v>28</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N27" s="7" t="s">
         <v>32</v>
@@ -2447,13 +2459,13 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="28">
         <v>12</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="29" t="s">
         <v>72</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -2472,7 +2484,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J28" s="8" t="s">
         <v>84</v>
@@ -2481,10 +2493,10 @@
         <v>26</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N28" s="7" t="s">
         <v>28</v>
@@ -2497,11 +2509,11 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="36"/>
-      <c r="B29" s="29">
+      <c r="A29" s="33"/>
+      <c r="B29" s="28">
         <v>13</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="29" t="s">
         <v>73</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -2520,7 +2532,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>85</v>
@@ -2532,7 +2544,7 @@
         <v>28</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N29" s="7" t="s">
         <v>30</v>
@@ -2545,11 +2557,11 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="36"/>
-      <c r="B30" s="29">
+      <c r="A30" s="33"/>
+      <c r="B30" s="28">
         <v>14</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="29" t="s">
         <v>74</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -2568,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J30" s="8" t="s">
         <v>85</v>
@@ -2580,7 +2592,7 @@
         <v>32</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N30" s="7" t="s">
         <v>28</v>
@@ -2593,11 +2605,11 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="36"/>
-      <c r="B31" s="29">
+      <c r="A31" s="33"/>
+      <c r="B31" s="28">
         <v>24</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="29" t="s">
         <v>75</v>
       </c>
       <c r="D31" s="7" t="s">
@@ -2616,7 +2628,7 @@
         <v>26</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>85</v>
@@ -2631,7 +2643,7 @@
         <v>30</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O31" s="7">
         <v>3</v>
@@ -2641,11 +2653,11 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="36"/>
-      <c r="B32" s="29">
+      <c r="A32" s="33"/>
+      <c r="B32" s="28">
         <v>31</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="31" t="s">
         <v>76</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -2664,7 +2676,7 @@
         <v>26</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>85</v>
@@ -2679,7 +2691,7 @@
         <v>59</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O32" s="7">
         <v>3</v>
@@ -2688,12 +2700,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="36"/>
-      <c r="B33" s="31">
+    <row r="33" spans="1:17">
+      <c r="A33" s="33"/>
+      <c r="B33" s="30">
         <v>25</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="31" t="s">
         <v>77</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -2712,7 +2724,7 @@
         <v>26</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>85</v>
@@ -2727,7 +2739,7 @@
         <v>28</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O33" s="7">
         <v>3</v>
@@ -2736,55 +2748,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
-      <c r="A34" s="26" t="s">
+    <row r="34" spans="1:17" s="48" customFormat="1">
+      <c r="A34" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="33">
+      <c r="B34" s="43">
         <v>19</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="7">
-        <v>1</v>
-      </c>
-      <c r="F34" s="7">
-        <v>0</v>
-      </c>
-      <c r="G34" s="7">
-        <v>0</v>
-      </c>
-      <c r="H34" s="7">
-        <v>1</v>
-      </c>
-      <c r="I34" s="19" t="s">
+      <c r="D34" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="45">
+        <v>1</v>
+      </c>
+      <c r="F34" s="45">
+        <v>0</v>
+      </c>
+      <c r="G34" s="45">
+        <v>0</v>
+      </c>
+      <c r="H34" s="45">
+        <v>1</v>
+      </c>
+      <c r="I34" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="J34" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="K34" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="L34" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="M34" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="N34" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="J34" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L34" s="7">
-        <v>0</v>
-      </c>
-      <c r="M34" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="O34" s="7">
+      <c r="O34" s="45">
         <v>3</v>
       </c>
-      <c r="P34" s="7">
-        <v>1</v>
-      </c>
+      <c r="P34" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2829,10 +2842,10 @@
       <c r="B1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="41">
-        <v>0</v>
-      </c>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="38">
+        <v>0</v>
+      </c>
+      <c r="D1" s="40" t="s">
         <v>89</v>
       </c>
       <c r="E1" s="9"/>
@@ -2852,8 +2865,8 @@
       <c r="B2" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="41"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -2964,7 +2977,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="13">
         <v>7</v>

</xml_diff>

<commit_message>
Update Controller's JumpType signal.
</commit_message>
<xml_diff>
--- a/doc/控制器.xlsx
+++ b/doc/控制器.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yifan/Desktop/SAOestCPU/doc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="寄存器定义" sheetId="2" r:id="rId1"/>
@@ -18,18 +23,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="111">
   <si>
     <t>寄存器</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -390,8 +395,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -680,6 +685,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -710,29 +734,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="常规 6" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -767,7 +772,7 @@
         <xdr:cNvPr id="3" name="直接连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FCE7D1A-8146-4B2C-8BF5-1F1E1E5E6C9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1FCE7D1A-8146-4B2C-8BF5-1F1E1E5E6C9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -817,7 +822,7 @@
         <xdr:cNvPr id="5" name="直接连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2262EF2A-6BE7-4BAE-B7BB-F24298545F56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2262EF2A-6BE7-4BAE-B7BB-F24298545F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1114,20 +1119,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.58203125" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1135,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1143,7 +1148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1159,7 +1164,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1167,7 +1172,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1175,7 +1180,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>106</v>
       </c>
@@ -1183,7 +1188,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>107</v>
       </c>
@@ -1198,17 +1203,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P22" sqref="P22"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="8.83203125" style="7"/>
     <col min="4" max="4" width="10.1640625" style="7" customWidth="1"/>
@@ -1224,37 +1229,37 @@
     <col min="17" max="17" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-    </row>
-    <row r="3" spans="1:17" ht="28">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+    </row>
+    <row r="3" spans="1:17" ht="28" x14ac:dyDescent="0.2">
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1273,10 +1278,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="37"/>
+      <c r="K3" s="44"/>
       <c r="L3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1294,8 +1299,8 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="26">
@@ -1344,8 +1349,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="33"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="40"/>
       <c r="B5" s="28">
         <v>2</v>
       </c>
@@ -1392,8 +1397,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="33"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="40"/>
       <c r="B6" s="28">
         <v>3</v>
       </c>
@@ -1440,8 +1445,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="33"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="40"/>
       <c r="B7" s="28">
         <v>4</v>
       </c>
@@ -1488,8 +1493,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="33"/>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="40"/>
       <c r="B8" s="28">
         <v>23</v>
       </c>
@@ -1536,8 +1541,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="33"/>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="40"/>
       <c r="B9" s="30">
         <v>29</v>
       </c>
@@ -1584,8 +1589,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="39" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="28">
@@ -1634,8 +1639,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="33"/>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="40"/>
       <c r="B11" s="30">
         <v>20</v>
       </c>
@@ -1682,8 +1687,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="39" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="28">
@@ -1732,8 +1737,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="33"/>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="40"/>
       <c r="B13" s="28">
         <v>22</v>
       </c>
@@ -1780,8 +1785,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="33"/>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="40"/>
       <c r="B14" s="30">
         <v>30</v>
       </c>
@@ -1828,8 +1833,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="32" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="28">
@@ -1878,8 +1883,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="33"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="40"/>
       <c r="B16" s="28">
         <v>7</v>
       </c>
@@ -1926,8 +1931,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="33"/>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="40"/>
       <c r="B17" s="28">
         <v>8</v>
       </c>
@@ -1974,8 +1979,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="33"/>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="40"/>
       <c r="B18" s="28">
         <v>9</v>
       </c>
@@ -2022,8 +2027,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="33"/>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="40"/>
       <c r="B19" s="28">
         <v>11</v>
       </c>
@@ -2070,8 +2075,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="33"/>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="40"/>
       <c r="B20" s="28">
         <v>26</v>
       </c>
@@ -2118,8 +2123,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="33"/>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="40"/>
       <c r="B21" s="30">
         <v>27</v>
       </c>
@@ -2166,8 +2171,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="32" t="s">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="39" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="28">
@@ -2209,15 +2214,15 @@
       <c r="N22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="O22" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P22" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="33"/>
+      <c r="O22" s="7">
+        <v>0</v>
+      </c>
+      <c r="P22" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="40"/>
       <c r="B23" s="30">
         <v>28</v>
       </c>
@@ -2257,15 +2262,15 @@
       <c r="N23" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="O23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P23" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="32" t="s">
+      <c r="O23" s="7">
+        <v>0</v>
+      </c>
+      <c r="P23" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="39" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="28">
@@ -2314,8 +2319,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="33"/>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="40"/>
       <c r="B25" s="28">
         <v>16</v>
       </c>
@@ -2362,8 +2367,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="33"/>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="40"/>
       <c r="B26" s="28">
         <v>17</v>
       </c>
@@ -2410,8 +2415,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="33"/>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="40"/>
       <c r="B27" s="30">
         <v>18</v>
       </c>
@@ -2458,8 +2463,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="32" t="s">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="39" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="28">
@@ -2508,8 +2513,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="33"/>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="40"/>
       <c r="B29" s="28">
         <v>13</v>
       </c>
@@ -2556,8 +2561,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="33"/>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="40"/>
       <c r="B30" s="28">
         <v>14</v>
       </c>
@@ -2604,8 +2609,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="33"/>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="40"/>
       <c r="B31" s="28">
         <v>24</v>
       </c>
@@ -2652,8 +2657,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="33"/>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="40"/>
       <c r="B32" s="28">
         <v>31</v>
       </c>
@@ -2700,8 +2705,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
-      <c r="A33" s="33"/>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="40"/>
       <c r="B33" s="30">
         <v>25</v>
       </c>
@@ -2748,56 +2753,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="48" customFormat="1">
-      <c r="A34" s="42" t="s">
+    <row r="34" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="43">
+      <c r="B34" s="33">
         <v>19</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="45">
-        <v>1</v>
-      </c>
-      <c r="F34" s="45">
-        <v>0</v>
-      </c>
-      <c r="G34" s="45">
-        <v>0</v>
-      </c>
-      <c r="H34" s="45">
-        <v>1</v>
-      </c>
-      <c r="I34" s="46" t="s">
+      <c r="D34" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="35">
+        <v>1</v>
+      </c>
+      <c r="F34" s="35">
+        <v>0</v>
+      </c>
+      <c r="G34" s="35">
+        <v>0</v>
+      </c>
+      <c r="H34" s="35">
+        <v>1</v>
+      </c>
+      <c r="I34" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="J34" s="47" t="s">
+      <c r="J34" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="K34" s="45" t="s">
+      <c r="K34" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="L34" s="45" t="s">
+      <c r="L34" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="M34" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="N34" s="45" t="s">
+      <c r="M34" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="N34" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="O34" s="45">
+      <c r="O34" s="35">
         <v>3</v>
       </c>
-      <c r="P34" s="45">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="45"/>
+      <c r="P34" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2821,31 +2826,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29" customHeight="1">
+    <row r="1" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="38">
-        <v>0</v>
-      </c>
-      <c r="D1" s="40" t="s">
+      <c r="C1" s="45">
+        <v>0</v>
+      </c>
+      <c r="D1" s="47" t="s">
         <v>89</v>
       </c>
       <c r="E1" s="9"/>
@@ -2858,15 +2863,15 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="39.5" customHeight="1">
+    <row r="2" spans="1:13" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -2877,7 +2882,7 @@
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>51</v>
       </c>
@@ -2891,7 +2896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>52</v>
       </c>
@@ -2905,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>54</v>
       </c>
@@ -2919,7 +2924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>55</v>
       </c>
@@ -2933,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>57</v>
       </c>
@@ -2947,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>58</v>
       </c>
@@ -2961,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>60</v>
       </c>
@@ -2975,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>108</v>
       </c>
@@ -2989,7 +2994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>94</v>
       </c>
@@ -3000,7 +3005,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="12">
         <v>1</v>
@@ -3009,7 +3014,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="13">
         <v>2</v>
@@ -3030,20 +3035,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
@@ -3051,7 +3056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
@@ -3059,7 +3064,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
@@ -3067,7 +3072,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
@@ -3075,7 +3080,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3083,7 +3088,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -3091,7 +3096,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>45</v>
       </c>
@@ -3099,7 +3104,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
@@ -3107,7 +3112,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
@@ -3123,20 +3128,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="210" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="8"/>
+    <col min="2" max="2" width="10.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>99</v>
       </c>
@@ -3144,7 +3149,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>100</v>
       </c>
@@ -3152,7 +3157,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>102</v>
       </c>
@@ -3160,7 +3165,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>101</v>
       </c>
@@ -3168,7 +3173,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>104</v>
       </c>

</xml_diff>